<commit_message>
Clean: the options.js have refactored.
</commit_message>
<xml_diff>
--- a/IndexedDB structure.xlsx
+++ b/IndexedDB structure.xlsx
@@ -502,32 +502,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -535,18 +535,18 @@
         <v>9</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:8">
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="C7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="C8" s="8" t="s">
         <v>9</v>
       </c>
@@ -557,7 +557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -565,7 +565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="7" t="s">
         <v>3</v>
       </c>
@@ -582,12 +582,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" s="7" t="s">
         <v>7</v>
       </c>
@@ -598,12 +598,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>14</v>
       </c>

</xml_diff>